<commit_message>
Creates first sitetracker demo testcase
</commit_message>
<xml_diff>
--- a/test cases/sitetracker-demo.xlsx
+++ b/test cases/sitetracker-demo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repo\sitetracker-demo\test cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9971D5E2-B0DF-4F26-96E4-AAD742AC7EC1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B539153-790A-4BA5-87B0-0FACE7CCC1B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="62">
   <si>
     <t>ID</t>
   </si>
@@ -113,12 +113,6 @@
 searchButton: //button [@data-testid="facebar_search_button" ]</t>
   </si>
   <si>
-    <t>Añadir cancion</t>
-  </si>
-  <si>
-    <t>Tener usuario y contrase;a validos, y browser chrome instalado.</t>
-  </si>
-  <si>
     <t>Busuqeda y Filtro en Amazón</t>
   </si>
   <si>
@@ -198,13 +192,6 @@
   </si>
   <si>
     <t>Edit row &lt;row_number&gt; in preview pane</t>
-  </si>
-  <si>
-    <t>Label: Larry Page
-Website: https://google.com
-Phone number:(555)-755-6575
-Date Time: Jan 01, 2022 12:57 PM
-Balance: 770.54</t>
   </si>
   <si>
     <t>Assert third row carries changes</t>
@@ -253,6 +240,64 @@
 specificationTab: css="[id='specification__item']"
 exampleInput: name="example"
 openInPlaygroundBtn: linkText="Open in Playground"</t>
+  </si>
+  <si>
+    <t>ComponentPage:
+openInPlaygroundBtn: linkText="Open in Playground"
+PlayGroundPage:
+header: css="[title='Data Table with Inline Edit']"
+projectHeader: xpath="//h1[@slot='title' and .='Project']"
+projectFilesHeader: xpath="//h1[@slot='title' and .='Project Files']"
+editingHeader: xpath="//h1[contains(@class, 'title') and contains(.,'Editing')]"
+previewHeader: xpath="//h1[contains(@class, 'title') and .='Preview']"
+dataTbl: css="table.slds-table_edit"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PlayGroundPage
+dataTbl: css="table.slds-table_edit"
+(dyn) dataRow: xpath="//table//tr[3]"
+(dyn) labelCol: xpath="./th[@data-label='Label']"
+(dyn) labelColEditBtn: xpath=".//button"
+(dyn) labelColEditTxt: name="dt-inline-edit-text"
+(dyn) labelColHeader: xpath=".//th[@aria-label='Label']"
+//website elements
+(dyn) websiteCol: xpath="./td[@data-label='Website']"
+(dyn) websiteColEditBtn: xpath=".//button"
+(dyn) websiteColEditTxt: name="dt-inline-edit-url"
+(dyn) websiteColHeader: xpath=".//th[@aria-label='Website']"
+//Phone elements
+(dyn) phoneCol: xpath="./td[@data-label='Phone']"
+(dyn) phoneColEditBtn: xpath=".//button"
+(dyn) phoneColEditTxt: name="dt-inline-edit-phone"
+(dyn) phoneColHeader: xpath=".//th[@aria-label='Website']"
+</t>
+  </si>
+  <si>
+    <t>//closeAt elements
+(dyn) closeAtCol: xpath="./td[@data-label='CloseAt']"
+(dyn) closeAtColEditBtn: xpath=".//button"
+(dyn) closeAtDateColEditTxt: xpath="//label[.='Date']/following-sibling::*/input"
+(dyn) closeAtTimeColEditTxt: xpath="//label[.='Time']/following-sibling::*/input"
+(dyn) closeAtColHeader: xpath=".//th[@aria-label='CloseAt']"
+//Balance elements
+(dyn) balanceCol: xpath="./td[@data-label='Balance']"
+(dyn) balanceColEditBtn: xpath=".//button"
+(dyn) balanceColEditTxt: name="dt-inline-edit-currency"
+(dyn) balanceColHeader: xpath=".//th[@aria-label='Balance']"</t>
+  </si>
+  <si>
+    <t>the user should be capable of editing a datatable inline</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>&lt;row_number&gt;: 3
+&lt;Label&gt;: Larry Page
+&lt;Website&gt;: https://google.com
+&lt;Phone number:(555)-755-6575
+&lt;Date Time&gt;: Jan 01, 2022 12:57 PM
+&lt;Balance&gt;: 770.54</t>
   </si>
 </sst>
 </file>
@@ -308,7 +353,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -323,12 +368,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -358,6 +418,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -679,18 +746,18 @@
       <selection activeCell="C1" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="4.33203125" customWidth="1"/>
-    <col min="2" max="3" width="31.33203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="30.5546875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="67.88671875" customWidth="1"/>
-    <col min="6" max="6" width="21.109375" customWidth="1"/>
+    <col min="1" max="1" width="4.28515625" customWidth="1"/>
+    <col min="2" max="3" width="31.28515625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="30.5703125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="67.85546875" customWidth="1"/>
+    <col min="6" max="6" width="21.140625" customWidth="1"/>
     <col min="7" max="7" width="29" customWidth="1"/>
-    <col min="8" max="26" width="10.6640625" customWidth="1"/>
+    <col min="8" max="26" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="14.4">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -706,13 +773,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="14.4">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -729,61 +796,61 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="57.6">
+    <row r="7" spans="1:6" ht="60">
       <c r="A7">
         <v>1</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F7" s="9"/>
     </row>
-    <row r="8" spans="1:6" ht="100.8">
+    <row r="8" spans="1:6" ht="105">
       <c r="A8">
         <v>2</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D8" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="E8" s="7" t="s">
-        <v>38</v>
-      </c>
       <c r="F8" s="9"/>
     </row>
-    <row r="9" spans="1:6" ht="28.8">
+    <row r="9" spans="1:6" ht="30">
       <c r="A9">
         <v>4</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D9" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="E9" s="11" t="s">
-        <v>39</v>
-      </c>
       <c r="F9" s="9"/>
     </row>
-    <row r="10" spans="1:6" ht="14.4">
+    <row r="10" spans="1:6">
       <c r="A10" s="4">
         <v>5</v>
       </c>
@@ -793,7 +860,7 @@
       <c r="E10" s="9"/>
       <c r="F10" s="9"/>
     </row>
-    <row r="11" spans="1:6" ht="14.4">
+    <row r="11" spans="1:6">
       <c r="A11" s="4"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -801,7 +868,7 @@
       <c r="E11" s="9"/>
       <c r="F11" s="9"/>
     </row>
-    <row r="12" spans="1:6" ht="14.4">
+    <row r="12" spans="1:6">
       <c r="A12" s="4">
         <v>6</v>
       </c>
@@ -824,23 +891,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55E53062-28D7-4895-A4C5-0E934E6B8F13}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD11"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
     <col min="2" max="2" width="21" style="2" customWidth="1"/>
     <col min="3" max="3" width="42" style="2" customWidth="1"/>
     <col min="4" max="4" width="47" style="2" customWidth="1"/>
-    <col min="5" max="5" width="63.6640625" customWidth="1"/>
-    <col min="6" max="6" width="21.109375" customWidth="1"/>
+    <col min="5" max="5" width="63.7109375" customWidth="1"/>
+    <col min="6" max="6" width="53.140625" customWidth="1"/>
     <col min="7" max="7" width="29" customWidth="1"/>
-    <col min="8" max="26" width="10.6640625" customWidth="1"/>
+    <col min="8" max="26" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="14.4">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -856,13 +923,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>25</v>
+        <v>59</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="14.4">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15" customHeight="1">
+      <c r="C3" s="7"/>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -879,101 +949,107 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="100.8">
+    <row r="7" spans="1:6" ht="105">
       <c r="A7">
         <v>1</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>43</v>
-      </c>
       <c r="E7" s="7" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F7" s="9"/>
     </row>
-    <row r="8" spans="1:6" ht="216">
+    <row r="8" spans="1:6" ht="225">
       <c r="A8">
         <v>2</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>46</v>
-      </c>
       <c r="E8" s="8" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F8" s="9"/>
     </row>
-    <row r="9" spans="1:6" ht="201.6">
+    <row r="9" spans="1:6" ht="225.75" thickBot="1">
       <c r="A9">
         <v>3</v>
       </c>
       <c r="B9" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E9" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>58</v>
-      </c>
       <c r="F9" s="9"/>
     </row>
-    <row r="10" spans="1:6" ht="84" customHeight="1">
+    <row r="10" spans="1:6" ht="180.75" thickBot="1">
       <c r="A10">
         <v>4</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E10" s="9"/>
+        <v>50</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>56</v>
+      </c>
       <c r="F10" s="9"/>
     </row>
-    <row r="11" spans="1:6" ht="84" customHeight="1">
+    <row r="11" spans="1:6" ht="270.75" thickBot="1">
       <c r="A11" s="4">
         <v>5</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-    </row>
-    <row r="12" spans="1:6" ht="14.4">
+        <v>61</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" s="4"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
-      <c r="D12" s="7"/>
+      <c r="D12" s="11"/>
       <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-    </row>
-    <row r="13" spans="1:6" ht="14.4">
+      <c r="F12" s="15"/>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" s="4">
         <v>6</v>
       </c>
@@ -997,19 +1073,19 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
     <col min="2" max="2" width="21" style="2" customWidth="1"/>
     <col min="3" max="3" width="42" style="2" customWidth="1"/>
     <col min="4" max="4" width="47" style="2" customWidth="1"/>
-    <col min="5" max="5" width="63.6640625" customWidth="1"/>
-    <col min="6" max="6" width="21.109375" customWidth="1"/>
+    <col min="5" max="5" width="63.7109375" customWidth="1"/>
+    <col min="6" max="6" width="21.140625" customWidth="1"/>
     <col min="7" max="7" width="29" customWidth="1"/>
-    <col min="8" max="26" width="10.6640625" customWidth="1"/>
+    <col min="8" max="26" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.4">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1031,7 +1107,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="14.4">
+    <row r="6" spans="1:5">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -1048,7 +1124,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="72">
+    <row r="7" spans="1:5" ht="75">
       <c r="A7">
         <v>1</v>
       </c>
@@ -1065,7 +1141,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="129.6">
+    <row r="8" spans="1:5" ht="135">
       <c r="A8">
         <v>2</v>
       </c>
@@ -1082,7 +1158,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="100.8">
+    <row r="9" spans="1:5" ht="105">
       <c r="A9">
         <v>3</v>
       </c>
@@ -1113,7 +1189,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="14.4">
+    <row r="11" spans="1:5">
       <c r="A11" s="4">
         <v>5</v>
       </c>
@@ -1121,12 +1197,12 @@
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
     </row>
-    <row r="12" spans="1:5" ht="14.4">
+    <row r="12" spans="1:5">
       <c r="A12" s="4"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
     </row>
-    <row r="13" spans="1:5" ht="14.4">
+    <row r="13" spans="1:5">
       <c r="A13" s="4">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
Adds Sitetracker demo pages
</commit_message>
<xml_diff>
--- a/test cases/sitetracker-demo.xlsx
+++ b/test cases/sitetracker-demo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repo\sitetracker-demo\test cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B539153-790A-4BA5-87B0-0FACE7CCC1B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A620F7E-F558-446A-8AB8-668E842FA72F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="0" windowWidth="16860" windowHeight="15450" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="3" r:id="rId1"/>
@@ -172,9 +172,6 @@
     <t>URL: https://developer.salesforce.com/docs/component-library/documentation/en/48.0/lwc</t>
   </si>
   <si>
-    <t>Search for &lt;component&gt; in Component Reference tab</t>
-  </si>
-  <si>
     <t>&lt;component&gt; is listed in the left nav menu</t>
   </si>
   <si>
@@ -240,17 +237,6 @@
 specificationTab: css="[id='specification__item']"
 exampleInput: name="example"
 openInPlaygroundBtn: linkText="Open in Playground"</t>
-  </si>
-  <si>
-    <t>ComponentPage:
-openInPlaygroundBtn: linkText="Open in Playground"
-PlayGroundPage:
-header: css="[title='Data Table with Inline Edit']"
-projectHeader: xpath="//h1[@slot='title' and .='Project']"
-projectFilesHeader: xpath="//h1[@slot='title' and .='Project Files']"
-editingHeader: xpath="//h1[contains(@class, 'title') and contains(.,'Editing')]"
-previewHeader: xpath="//h1[contains(@class, 'title') and .='Preview']"
-dataTbl: css="table.slds-table_edit"</t>
   </si>
   <si>
     <t xml:space="preserve">PlayGroundPage
@@ -298,6 +284,22 @@
 &lt;Phone number:(555)-755-6575
 &lt;Date Time&gt;: Jan 01, 2022 12:57 PM
 &lt;Balance&gt;: 770.54</t>
+  </si>
+  <si>
+    <t>select &lt;component&gt; from &lt;path&gt; in left nav</t>
+  </si>
+  <si>
+    <t>ComponentPage:
+exampleInput: name="example"
+(dyn) inlineEditLinkText: partialLinkText="InlineEdit"
+openInPlaygroundBtn: linkText="Open in Playground"
+PlayGroundPage:
+header: css="[title='Data Table with Inline Edit']"
+projectHeader: xpath="//h1[@slot='title' and .='Project']"
+projectFilesHeader: xpath="//h1[@slot='title' and .='Project Files']"
+editingHeader: xpath="//h1[contains(@class, 'title') and contains(.,'Editing')]"
+previewHeader: xpath="//h1[contains(@class, 'title') and .='Preview']"
+dataTbl: css="table.slds-table_edit"</t>
   </si>
 </sst>
 </file>
@@ -891,8 +893,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55E53062-28D7-4895-A4C5-0E934E6B8F13}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="B9" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -923,10 +925,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15" customHeight="1">
@@ -963,7 +965,7 @@
         <v>41</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F7" s="9"/>
     </row>
@@ -972,16 +974,16 @@
         <v>2</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="D8" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>44</v>
-      </c>
       <c r="E8" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F8" s="9"/>
     </row>
@@ -990,34 +992,34 @@
         <v>3</v>
       </c>
       <c r="B9" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>53</v>
-      </c>
       <c r="E9" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F9" s="9"/>
     </row>
-    <row r="10" spans="1:6" ht="180.75" thickBot="1">
+    <row r="10" spans="1:6" ht="210.75" thickBot="1">
       <c r="A10">
         <v>4</v>
       </c>
       <c r="B10" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>47</v>
-      </c>
       <c r="D10" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="F10" s="9"/>
     </row>
@@ -1026,19 +1028,19 @@
         <v>5</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>49</v>
-      </c>
       <c r="D11" s="12" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:6">

</xml_diff>

<commit_message>
Adds select component type and edit row functionality
</commit_message>
<xml_diff>
--- a/test cases/sitetracker-demo.xlsx
+++ b/test cases/sitetracker-demo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repo\sitetracker-demo\test cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A620F7E-F558-446A-8AB8-668E842FA72F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B445099-D9F7-4B96-A3A2-52B956CF642B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1560" yWindow="0" windowWidth="16860" windowHeight="15450" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -893,8 +893,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55E53062-28D7-4895-A4C5-0E934E6B8F13}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B9" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="E10" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1"/>

</xml_diff>